<commit_message>
Fix Google Doc parsing, add EST timezone, update UI and README
- GoogleDocParserService: rewrite parser to support both multi-line and
  single-line doc formats; match 'Email N: description' headers with prefix
  regex; strip Unicode invisibles; split inline subject/body at greeting
- ExcelImportService: add M/d/yyyy H:mm:ss date format (with seconds);
  improve import logging (column indices, sections parsed, jobs created)
- CampaignService: simplify launch() — no longer requires templates,
  only checks for enrolled contacts
- campaign-detail: remove Email Templates tab; UI now has 3 tabs:
  Overview, Contacts, Email Jobs
- manifest.yml: add TZ=America/New_York so server runs on EST and
  spreadsheet dates don't need UTC conversion
- README: document screen layout (3 tabs), date format table, EST timezone
  note, Google Doc format examples, opt-out behavior, and CF deploy steps

Co-Authored-By: Claude Sonnet 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/examples/sample.xlsx
+++ b/examples/sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sameerhashmi/workspace/CC App/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D32196D-2288-E442-9050-230B1B123DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904F271E-4FB4-8B40-8C6B-4BC058313F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="89520" yWindow="4820" windowWidth="32060" windowHeight="20680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52280" yWindow="1180" windowWidth="32060" windowHeight="20680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>company</t>
   </si>
@@ -86,6 +86,15 @@
   </si>
   <si>
     <t>CISO</t>
+  </si>
+  <si>
+    <t>sheet1</t>
+  </si>
+  <si>
+    <t>Sheet2</t>
+  </si>
+  <si>
+    <t>Sheet 3</t>
   </si>
 </sst>
 </file>
@@ -457,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -471,7 +480,7 @@
     <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -485,7 +494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -498,8 +507,11 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -511,6 +523,14 @@
       </c>
       <c r="D3" t="s">
         <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -527,7 +547,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>